<commit_message>
Fix coordinate and rotation of CN1 and U1 in the CPL file
</commit_message>
<xml_diff>
--- a/MeishinoCH552_CPL_JLCSMT.xlsx
+++ b/MeishinoCH552_CPL_JLCSMT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akita/Desktop/PCB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\JLCPCB\2022_07\MeishinoCH552\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C27230-F928-084E-AFEC-CE3BB2F62AAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296FC9B8-3986-4B35-B8C9-DFB6EB4C3B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="10500" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18168" yWindow="0" windowWidth="11712" windowHeight="25200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,19 +444,19 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" customHeight="1">
+    <row r="1" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,7 +473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1">
+    <row r="2" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -490,7 +490,7 @@
         <v>-90</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
+    <row r="3" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -507,7 +507,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
+    <row r="4" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -515,16 +515,16 @@
         <v>25.4</v>
       </c>
       <c r="C4" s="2">
-        <v>-6.5</v>
+        <v>-5</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="2">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -541,7 +541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -558,7 +558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -575,7 +575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -592,7 +592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -609,7 +609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="13.8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -643,7 +643,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="13.8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="13.8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -677,7 +677,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="13.8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -691,7 +691,7 @@
         <v>18</v>
       </c>
       <c r="E14" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>